<commit_message>
End of First Sprint
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -3,24 +3,30 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="24" documentId="11_F25DC773A252ABEACE02EC641B9B50FC5BDE58A2" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{B7861868-0497-481B-899E-0B16F3B32AEE}"/>
+  <xr:revisionPtr revIDLastSave="169" documentId="11_F25DC773A252ABEACE02EC641B9B50FC5BDE58A2" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{225F7DDC-F013-4453-925B-D7FFE9EF9B14}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="270" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>Tasks</t>
   </si>
@@ -31,9 +37,6 @@
     <t>Point allocation</t>
   </si>
   <si>
-    <t>Sprint number</t>
-  </si>
-  <si>
     <t>Research components</t>
   </si>
   <si>
@@ -46,15 +49,6 @@
     <t>Design head of arm</t>
   </si>
   <si>
-    <t>Construct head of arm</t>
-  </si>
-  <si>
-    <t>Test head of arm</t>
-  </si>
-  <si>
-    <t>Print arm body</t>
-  </si>
-  <si>
     <t>Design arm body</t>
   </si>
   <si>
@@ -64,7 +58,73 @@
     <t>Test arm body</t>
   </si>
   <si>
-    <t>Attach arm and head</t>
+    <t>Design app</t>
+  </si>
+  <si>
+    <t>Program individual movements</t>
+  </si>
+  <si>
+    <t>Program synchronised movements</t>
+  </si>
+  <si>
+    <t>Link movements to app buttons</t>
+  </si>
+  <si>
+    <t>Test app connection to arduino</t>
+  </si>
+  <si>
+    <t>Construct head</t>
+  </si>
+  <si>
+    <t>Test head</t>
+  </si>
+  <si>
+    <t>Get a wearable body mount</t>
+  </si>
+  <si>
+    <t>Design housing for the main electronics</t>
+  </si>
+  <si>
+    <t>Construct housing</t>
+  </si>
+  <si>
+    <t>Attatch arm, head, mount and housing</t>
+  </si>
+  <si>
+    <t>Make any necessary adjustments to apparatus</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>XS</t>
+  </si>
+  <si>
+    <t>XL</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Code app output</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>Sprint Avg:</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>Test overall performance of apparatus</t>
   </si>
 </sst>
 </file>
@@ -88,15 +148,39 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -113,13 +197,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,20 +502,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -423,67 +526,301 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="9"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <f>SUM(C2:C4)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <f>SUM(C5:C7,C11:C12)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
+      </c>
+      <c r="E4" s="6">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <f>SUM(C8:C10,C13:C15)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="E5" s="7">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <f>SUM(C16:C22)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2">
+        <f>SUM(F2:F5)</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>14</v>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="2">
+        <f>SUM(C2:C22)</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24">
+        <f>C23/4</f>
+        <v>18.75</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="F2 F5" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>